<commit_message>
Status for 9th april - Func and NFT
</commit_message>
<xml_diff>
--- a/Daily Status update Report 09-04-2020.xlsx
+++ b/Daily Status update Report 09-04-2020.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="146">
   <si>
     <t>Sr.No</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>Started with Test Execution plan for PT; Discussed review comments with Pruthvi on Trade flow test cases; Had internal team call for functional walk through of settlement module; Completed reverse KT/open questions with Niranjan on the Modified Trade Flow</t>
+  </si>
+  <si>
+    <t>Team Discussion and Use case document understanding for Collateral and Settlement session with non functional team</t>
   </si>
 </sst>
 </file>
@@ -6191,7 +6194,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7519,19 +7522,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.125" style="25" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="9.875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="25" customWidth="1"/>
-    <col min="7" max="7" width="208" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="6.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="81.75" style="25" customWidth="1"/>
     <col min="8" max="26" width="7.625" style="25" customWidth="1"/>
     <col min="27" max="16384" width="12.625" style="25"/>
   </cols>
@@ -7578,7 +7578,9 @@
       <c r="F2" s="18">
         <v>0.75</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="26" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -7599,7 +7601,9 @@
       <c r="F3" s="18">
         <v>0.75</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="28" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -7620,7 +7624,9 @@
       <c r="F4" s="18">
         <v>0.77083333333333337</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="26" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -7641,7 +7647,9 @@
       <c r="F5" s="18">
         <v>0.77083333333333337</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="26" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -7662,7 +7670,9 @@
       <c r="F6" s="18">
         <v>0.75</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -7683,7 +7693,9 @@
       <c r="F7" s="18">
         <v>0.75</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -7704,7 +7716,9 @@
       <c r="F8" s="18">
         <v>0.75</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="26" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -7725,7 +7739,9 @@
       <c r="F9" s="18">
         <v>0.75</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
@@ -7838,7 +7854,9 @@
       <c r="F14" s="38">
         <v>0.77083333333333337</v>
       </c>
-      <c r="G14" s="40"/>
+      <c r="G14" s="40" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>